<commit_message>
createCourseObj function, create Excel version of BCM course catalog
</commit_message>
<xml_diff>
--- a/Calendar.xlsx
+++ b/Calendar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Monday</t>
   </si>
@@ -142,9 +142,19 @@
     <t>5:00</t>
   </si>
   <si>
-    <t>GS-QC-6301
-9:00 - 10:30
-N315</t>
+    <t xml:space="preserve">GS-GS-6600 
+1:15-2:15 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS-GS-6400 
+2:30-3:30 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS-NE-6112 
+09:00-12:00 
+N.0150.01 NRI </t>
   </si>
 </sst>
 </file>
@@ -526,154 +536,186 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>42</v>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>16</v>
       </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>18</v>
       </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>35</v>
       </c>
+      <c r="B32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
@@ -706,9 +748,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="F6:F12"/>
+  <mergeCells count="6">
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="E28:E32"/>
+    <mergeCell ref="C6:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add function to detect conflicting courses.
</commit_message>
<xml_diff>
--- a/Calendar.xlsx
+++ b/Calendar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Monday</t>
   </si>
@@ -142,19 +142,49 @@
     <t>5:00</t>
   </si>
   <si>
-    <t xml:space="preserve">GS-GS-6600 
-1:15-2:15 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS-GS-6400 
-2:30-3:30 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS-NE-6112 
-09:00-12:00 
-N.0150.01 NRI </t>
+    <t>5:15</t>
+  </si>
+  <si>
+    <t>5:30</t>
+  </si>
+  <si>
+    <t>5:45</t>
+  </si>
+  <si>
+    <t>6:00</t>
+  </si>
+  <si>
+    <t>6:15</t>
+  </si>
+  <si>
+    <t>6:30</t>
+  </si>
+  <si>
+    <t>6:45</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>7:15</t>
+  </si>
+  <si>
+    <t>7:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS-CP-6203 
+11:00-1:00
+N304 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS-CC-6202 
+11:00-12:30 
+M616 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS-CC-6208 
+10:00-11:00 
+N311 </t>
   </si>
 </sst>
 </file>
@@ -489,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -536,186 +566,177 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="C19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="C20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
@@ -747,14 +768,64 @@
         <v>41</v>
       </c>
     </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="E28:E32"/>
-    <mergeCell ref="C6:C18"/>
+    <mergeCell ref="C14:C22"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="F10:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create Function to parse PDFs for course names.
</commit_message>
<xml_diff>
--- a/Calendar.xlsx
+++ b/Calendar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Monday</t>
   </si>
@@ -185,6 +185,11 @@
     <t xml:space="preserve">GS-CC-6208 
 10:00-11:00 
 N311 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS-QC-6301 
+09:00-10:30 
+</t>
   </si>
 </sst>
 </file>
@@ -566,35 +571,43 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>11</v>
       </c>
+      <c r="B8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
+      <c r="B9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -819,13 +832,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="C14:C22"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="E14:E20"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="D10:D14"/>
     <mergeCell ref="F10:F14"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="F6:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add function that adds link to location of buildings.
</commit_message>
<xml_diff>
--- a/Calendar.xlsx
+++ b/Calendar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Monday</t>
   </si>
@@ -172,24 +172,12 @@
     <t>7:30</t>
   </si>
   <si>
-    <t xml:space="preserve">GS-CP-6203 
-11:00-1:00
-N304 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS-CC-6202 
-11:00-12:30 
-M616 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS-CC-6208 
-10:00-11:00 
-N311 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS-QC-6301 
-09:00-10:30 
-</t>
+    <t xml:space="preserve">N310 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS-DD-6208 
+1:00-2:30 
+N310 </t>
   </si>
 </sst>
 </file>
@@ -571,165 +559,134 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
+      <c r="C23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
+      <c r="C24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>28</v>
       </c>
+      <c r="C25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
+      <c r="C26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
+      <c r="C27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>31</v>
       </c>
+      <c r="C28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
@@ -832,16 +789,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C14:C22"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="F6:F12"/>
+  <mergeCells count="2">
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="E22:E28"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C28" r:id="rId1" display="https://www.google.com/maps/dir/Fondren+Gardens,+Houston,+TX/6565+Fannin+St,+Houston,+TX+77030/@29.6290837,-95.5114548,15.31z/data=!4m13!4m12!1m5!1m1!1s0x8640e9093d20ed91:0x82b6198af0aa9bee!2m2!1d-95.5012732!2d29.6263258!1m5!1m1!1s0x8640c071374b0fbd:0x4169184b828fca15!2m2!1d-95.3997225!2d29.7099079"/>
+    <hyperlink ref="E28" r:id="rId2" display="https://www.google.com/maps/dir/Fondren+Gardens,+Houston,+TX/6565+Fannin+St,+Houston,+TX+77030/@29.6290837,-95.5114548,15.31z/data=!4m13!4m12!1m5!1m1!1s0x8640e9093d20ed91:0x82b6198af0aa9bee!2m2!1d-95.5012732!2d29.6263258!1m5!1m1!1s0x8640c071374b0fbd:0x4169184b828fca15!2m2!1d-95.3997225!2d29.7099079"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>